<commit_message>
Initial commit - Velvet Lavender Invoice Generator
</commit_message>
<xml_diff>
--- a/Anainvoices.xlsx
+++ b/Anainvoices.xlsx
@@ -510,7 +510,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>#15</t>
+          <t>#16</t>
         </is>
       </c>
       <c r="D2" s="2" t="n">
@@ -557,7 +557,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>#15</t>
+          <t>#16</t>
         </is>
       </c>
       <c r="D3" s="2" t="n">

</xml_diff>